<commit_message>
Updating Data Transformation Practice Sheet
</commit_message>
<xml_diff>
--- a/Data Transformation Practice Sheet.xlsx
+++ b/Data Transformation Practice Sheet.xlsx
@@ -1,34 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\divya\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\divya\Documents\F_T_J_S\Excel Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C753AC8D-B7BD-4B13-9FD9-E15924F60257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9A62AD-E0AA-4AD4-8954-FB343C86AC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Original Data" sheetId="4" r:id="rId1"/>
-    <sheet name="Modified Sheet" sheetId="5" r:id="rId2"/>
+    <sheet name="Original Sales Data" sheetId="4" r:id="rId1"/>
+    <sheet name="Modified Sales Data" sheetId="5" r:id="rId2"/>
+    <sheet name="Question 13" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Modified Sheet'!$B$1:$F$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Original Data'!$A$1:$E$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Modified Sales Data'!$C$1:$G$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Original Sales Data'!$A$1:$E$6</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId3"/>
+    <pivotCache cacheId="15" r:id="rId4"/>
+    <pivotCache cacheId="19" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -167,18 +169,79 @@
   <si>
     <t>Lookup Values</t>
   </si>
+  <si>
+    <t>Total Sales</t>
+  </si>
+  <si>
+    <t>VLOOKUP</t>
+  </si>
+  <si>
+    <t>01-01-2023</t>
+  </si>
+  <si>
+    <t>HLOOKUP</t>
+  </si>
+  <si>
+    <t>Lookup Value</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Sample Variance</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Descriptive Statistic for Sales Amount</t>
+  </si>
+  <si>
+    <t>Month Number</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="[$£-809]#,##0.00;\-[$£-809]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$£-809]#,##0.00;\-[$£-809]#,##0.00"/>
+    <numFmt numFmtId="178" formatCode="[$-14009]yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,8 +288,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,8 +334,32 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -476,11 +577,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,7 +686,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
@@ -519,12 +693,9 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -532,81 +703,72 @@
     <xf numFmtId="166" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="178" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <font>
         <b val="0"/>
@@ -624,12 +786,161 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="178" formatCode="[$-14009]yyyy/mm/dd;@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.59999389629810485"/>
           <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="178" formatCode="[$-14009]yyyy/mm/dd;@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF009E47"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF009E47"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -685,7 +996,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="170" formatCode="[$£-809]#,##0.00;\-[$£-809]#,##0.00"/>
+      <numFmt numFmtId="167" formatCode="[$£-809]#,##0.00;\-[$£-809]#,##0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.59999389629810485"/>
@@ -815,7 +1126,63 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" indent="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" indent="0"/>
@@ -836,71 +1203,7 @@
       <alignment horizontal="center" indent="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF009E47"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF009E47"/>
-      </font>
+      <alignment horizontal="center" indent="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -936,7 +1239,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[807338d8-22f0-4999-8109-743bbbf40b99__9c53282b-9454-4b7c-9d49-4e665a13cb8e.xlsx]Modified Sheet!PivotTable5</c:name>
+    <c:name>[Data Transformation Practice Sheet.xlsx]Modified Sales Data!PivotTable5</c:name>
     <c:fmtId val="4"/>
   </c:pivotSource>
   <c:chart>
@@ -1107,7 +1410,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Modified Sheet'!$C$27</c:f>
+              <c:f>'Modified Sales Data'!$C$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1129,7 +1432,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Modified Sheet'!$B$28:$B$36</c:f>
+              <c:f>'Modified Sales Data'!$B$28:$B$36</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -1165,7 +1468,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Modified Sheet'!$C$28:$C$36</c:f>
+              <c:f>'Modified Sales Data'!$C$28:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1195,7 +1498,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Modified Sheet'!$D$27</c:f>
+              <c:f>'Modified Sales Data'!$D$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1217,7 +1520,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Modified Sheet'!$B$28:$B$36</c:f>
+              <c:f>'Modified Sales Data'!$B$28:$B$36</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
                 <c:lvl>
@@ -1253,7 +1556,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Modified Sheet'!$D$28:$D$36</c:f>
+              <c:f>'Modified Sales Data'!$D$28:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1618,7 +1921,556 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Sales Trend</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Modified Sales Data'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Modified Sales Data'!$C$2:$E$6</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>A</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>D</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>B</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>C</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>A</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>North</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>West</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>South</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>East</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>North</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2023-01-05</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2023-01-04</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2023-01-02</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2023-01-03</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2023-01-01</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Modified Sales Data'!$F$2:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-53AE-4E05-9964-A5006CF522CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Modified Sales Data'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Sales </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Modified Sales Data'!$C$2:$E$6</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>A</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>D</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>B</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>C</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>A</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>North</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>West</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>South</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>East</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>North</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2023-01-05</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2023-01-04</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2023-01-02</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2023-01-03</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2023-01-01</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Modified Sales Data'!$G$2:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>[$£-809]#,##0.00;\-[$£-809]#,##0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-53AE-4E05-9964-A5006CF522CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="227448096"/>
+        <c:axId val="227449536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="227448096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="227449536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="227449536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="227448096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2152,6 +3004,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$M$2" lockText="1" noThreeD="1"/>
 </file>
@@ -2249,23 +3617,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$M$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$M$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$M$22" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$M$22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$M$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$M$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$M$24" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$M$24" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$M$25" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$M$25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2273,11 +3641,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$M$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$M$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$M$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$M$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3597,7 +4965,7 @@
           <xdr:col>11</xdr:col>
           <xdr:colOff>577850</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3607,7 +4975,7 @@
                   <a14:compatExt spid="_x0000_s4097"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5723DCB4-EDA2-4B66-97B9-196D79DC35EF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3674,7 +5042,7 @@
                   <a14:compatExt spid="_x0000_s4098"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A91C2022-A937-4FF5-951B-0A9D8446F2EE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3741,7 +5109,7 @@
                   <a14:compatExt spid="_x0000_s4099"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C65B208-5E71-48EF-9EFD-C4E9525589A2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3808,7 +5176,7 @@
                   <a14:compatExt spid="_x0000_s4100"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47329774-5FAB-4592-9989-CA71CBCC02DE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3875,7 +5243,7 @@
                   <a14:compatExt spid="_x0000_s4101"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{516716CD-7CD3-4724-9396-AB3B80CF9C1E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3942,7 +5310,7 @@
                   <a14:compatExt spid="_x0000_s4102"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C3E985C-1992-48F2-8C37-B25E2D268CCF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4009,7 +5377,7 @@
                   <a14:compatExt spid="_x0000_s4103"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18D49C8D-5EBC-4329-9715-0F28B730C315}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4076,7 +5444,7 @@
                   <a14:compatExt spid="_x0000_s4104"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07A94264-B2A8-4825-9863-AB2CF3D8A945}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4143,7 +5511,7 @@
                   <a14:compatExt spid="_x0000_s4105"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75CAE080-8B6F-4130-92AF-2A868C0DFB6F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4210,7 +5578,7 @@
                   <a14:compatExt spid="_x0000_s4106"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4380B486-1CC7-410E-A0C2-9683E32961AB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4277,7 +5645,7 @@
                   <a14:compatExt spid="_x0000_s4107"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEBD4336-2166-46F5-A91F-BA13F3BED116}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4344,7 +5712,7 @@
                   <a14:compatExt spid="_x0000_s4108"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6413F3B2-4476-44FA-96B0-E8BC0FF0A5F0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4411,7 +5779,7 @@
                   <a14:compatExt spid="_x0000_s4109"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{484655A2-E5AC-4359-8688-E2AD20F7BF8D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4478,7 +5846,7 @@
                   <a14:compatExt spid="_x0000_s4110"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{488C21E9-026B-4E54-8567-E515C88991F2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4545,7 +5913,7 @@
                   <a14:compatExt spid="_x0000_s4111"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{699B1324-1EF2-4280-B9B1-4068ABA8E5B8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4612,7 +5980,7 @@
                   <a14:compatExt spid="_x0000_s4112"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88CA0D37-219C-47C2-9D8B-C9A660BD0811}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4679,7 +6047,7 @@
                   <a14:compatExt spid="_x0000_s4113"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CC8C416-466E-474B-8425-7173F8052D9A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4746,7 +6114,7 @@
                   <a14:compatExt spid="_x0000_s4114"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC626A7B-5687-4F87-92AA-B0309928337D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4813,7 +6181,7 @@
                   <a14:compatExt spid="_x0000_s4115"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FB839C4-2509-400E-90F4-F961DE6372C5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4893,6 +6261,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>307975</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>12699</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>168274</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFA241A2-E84D-600B-2345-13B1E6341233}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4903,7 +6307,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Divya Bha" refreshedDate="45512.52979803241" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="5" xr:uid="{40A7F8A3-AB29-421E-A1A2-E276BD4A20D9}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="C1:F6" sheet="Modified Sheet"/>
+    <worksheetSource ref="D1:G6" sheet="Modified Sales Data"/>
   </cacheSource>
   <cacheFields count="4">
     <cacheField name="Region" numFmtId="0">
@@ -4927,6 +6331,44 @@
     </cacheField>
     <cacheField name="Sales" numFmtId="166">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="100" maxValue="300"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Divya Bha" refreshedDate="45513.45101203704" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="5" xr:uid="{C2CB4490-21E8-4846-AA5B-2B5A4A611B00}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table4"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Date" numFmtId="0">
+      <sharedItems containsDate="1" containsMixedTypes="1" minDate="2023-01-01T00:00:00" maxDate="2023-01-02T00:00:00"/>
+    </cacheField>
+    <cacheField name="Region" numFmtId="0">
+      <sharedItems count="4">
+        <s v="North"/>
+        <s v="West"/>
+        <s v="South"/>
+        <s v="East"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Product" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Quantity" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10" maxValue="30"/>
+    </cacheField>
+    <cacheField name="Sales" numFmtId="167">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="100" maxValue="300"/>
+    </cacheField>
+    <cacheField name="Bonus" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="30"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -4972,8 +6414,53 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="5">
+  <r>
+    <s v="2023-01-05"/>
+    <x v="0"/>
+    <s v="A"/>
+    <n v="30"/>
+    <n v="300"/>
+    <n v="30"/>
+  </r>
+  <r>
+    <s v="2023-01-04"/>
+    <x v="1"/>
+    <s v="D"/>
+    <n v="25"/>
+    <n v="250"/>
+    <n v="25"/>
+  </r>
+  <r>
+    <s v="2023-01-02"/>
+    <x v="2"/>
+    <s v="B"/>
+    <n v="20"/>
+    <n v="200"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <s v="2023-01-03"/>
+    <x v="3"/>
+    <s v="C"/>
+    <n v="15"/>
+    <n v="150"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <d v="2023-01-01T00:00:00"/>
+    <x v="0"/>
+    <s v="A"/>
+    <n v="10"/>
+    <n v="100"/>
+    <n v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{968E4C5E-E1B8-4026-B5E9-5FAF1A2C35AF}" name="PivotTable5" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{968E4C5E-E1B8-4026-B5E9-5FAF1A2C35AF}" name="PivotTable5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="B27:D36" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -5046,20 +6533,20 @@
     <dataField name="Sum of Sales" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="7">
-    <format dxfId="13">
+    <format dxfId="30">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5071,7 +6558,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5083,7 +6570,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="25">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5095,7 +6582,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -5140,17 +6627,77 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{995C0C4E-B3E8-43A6-BB1F-56181EBE8375}" name="PivotTable6" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="167" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Sales" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{35466F57-6EB4-45A6-9916-BD3C7FE9F920}" name="Table4" displayName="Table4" ref="B1:G6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="B1:G6" xr:uid="{35466F57-6EB4-45A6-9916-BD3C7FE9F920}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2AF7987C-BB06-4FBD-BBEC-63F51A538296}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{89D56B67-F047-4E77-9A61-70D162A113F3}" name="Region" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{83DF1258-1270-4C8A-ACD6-20ABFCAD5355}" name="Product" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{63944184-22E7-44F5-A9B8-C94A48727087}" name="Quantity" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{33B57414-17A1-4BB6-A0D2-DC10BDFDC589}" name="Sales" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{A8B546A8-1D55-4976-8C3C-452403319223}" name="Bonus" dataDxfId="2">
-      <calculatedColumnFormula>IF(F2&gt;200,F2*0.1, 0)</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{35466F57-6EB4-45A6-9916-BD3C7FE9F920}" name="Table4" displayName="Table4" ref="B1:H6" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B1:H6" xr:uid="{35466F57-6EB4-45A6-9916-BD3C7FE9F920}"/>
+  <tableColumns count="7">
+    <tableColumn id="7" xr3:uid="{AE646EA1-703D-4777-B47D-DBD217CF1BCC}" name="Month Number" dataDxfId="0">
+      <calculatedColumnFormula>RIGHT(C2,2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="1" xr3:uid="{2AF7987C-BB06-4FBD-BBEC-63F51A538296}" name="Date" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{89D56B67-F047-4E77-9A61-70D162A113F3}" name="Region" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{83DF1258-1270-4C8A-ACD6-20ABFCAD5355}" name="Product" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{63944184-22E7-44F5-A9B8-C94A48727087}" name="Quantity" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{33B57414-17A1-4BB6-A0D2-DC10BDFDC589}" name="Sales" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{A8B546A8-1D55-4976-8C3C-452403319223}" name="Bonus" dataDxfId="17">
+      <calculatedColumnFormula>IF(G2&gt;200,G2*0.1, 0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5835,7 +7382,7 @@
     <sortCondition descending="1" ref="E2:E6"/>
   </sortState>
   <conditionalFormatting sqref="K2:K20">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6271,20 +7818,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C5FBA98-9226-4176-84A5-522169077450}">
-  <dimension ref="B1:S36"/>
+  <dimension ref="B1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="K13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.36328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" style="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6328125" style="35" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" style="19" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="13.453125" customWidth="1"/>
     <col min="10" max="10" width="4.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="51.6328125" bestFit="1" customWidth="1"/>
@@ -6296,127 +7843,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="F1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="32" t="s">
+    <row r="2" spans="2:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="51" t="str">
+        <f>RIGHT(C2,2)</f>
+        <v>05</v>
+      </c>
+      <c r="C2" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="E2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="27">
+      <c r="F2" s="25">
         <v>30</v>
       </c>
-      <c r="F2" s="38">
+      <c r="G2" s="32">
         <v>300</v>
       </c>
-      <c r="G2" s="29">
-        <f>IF(F2&gt;200,F2*0.1, 0)</f>
+      <c r="H2" s="27">
+        <f>IF(G2&gt;200,G2*0.1, 0)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B3" s="33" t="s">
+    <row r="3" spans="2:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="51" t="str">
+        <f t="shared" ref="B3:B5" si="0">RIGHT(C3,2)</f>
+        <v>04</v>
+      </c>
+      <c r="C3" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="D3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="E3" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="28">
+      <c r="F3" s="26">
         <v>25</v>
       </c>
-      <c r="F3" s="39">
+      <c r="G3" s="33">
         <v>250</v>
       </c>
-      <c r="G3" s="30">
-        <f t="shared" ref="G3:G6" si="0">IF(F3&gt;200,F3*0.1, 0)</f>
+      <c r="H3" s="28">
+        <f t="shared" ref="H3:H6" si="1">IF(G3&gt;200,G3*0.1, 0)</f>
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B4" s="34" t="s">
+    <row r="4" spans="2:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="51" t="str">
+        <f t="shared" si="0"/>
+        <v>02</v>
+      </c>
+      <c r="C4" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="22">
+      <c r="F4" s="21">
         <v>20</v>
       </c>
-      <c r="F4" s="40">
+      <c r="G4" s="34">
         <v>200</v>
       </c>
-      <c r="G4" s="31">
+      <c r="H4" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="51" t="str">
         <f t="shared" si="0"/>
+        <v>03</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="26">
+        <v>15</v>
+      </c>
+      <c r="G5" s="33">
+        <v>150</v>
+      </c>
+      <c r="H5" s="28">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B5" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="28">
-        <v>15</v>
-      </c>
-      <c r="F5" s="39">
-        <v>150</v>
-      </c>
-      <c r="G5" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="35">
+    <row r="6" spans="2:13" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="51" t="e">
+        <f>VALUE(MID(C6, 6, 2))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C6" s="53">
         <v>44927</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="22">
+      <c r="F6" s="21">
         <v>10</v>
       </c>
-      <c r="F6" s="40">
+      <c r="G6" s="34">
         <v>100</v>
       </c>
-      <c r="G6" s="31">
-        <f t="shared" si="0"/>
+      <c r="H6" s="29">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6434,12 +8004,6 @@
       <c r="M7" s="12"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
       <c r="I8" s="8"/>
       <c r="J8" s="16">
         <v>1</v>
@@ -6453,13 +8017,6 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="23">
-        <f>VLOOKUP(B9, $D$2:$G$6, 3, FALSE)</f>
-        <v>300</v>
-      </c>
       <c r="J9" s="16">
         <v>2</v>
       </c>
@@ -6472,13 +8029,15 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="23">
-        <f>VLOOKUP(B10, $D$2:$G$6, 3, FALSE)</f>
-        <v>200</v>
-      </c>
+      <c r="B10"/>
+      <c r="C10" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10"/>
       <c r="J10" s="16">
         <v>3</v>
       </c>
@@ -6491,7 +8050,19 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="I11" s="19"/>
+      <c r="B11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="18"/>
       <c r="J11" s="16">
         <v>4</v>
       </c>
@@ -6504,6 +8075,21 @@
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="22">
+        <f>VLOOKUP(B12, $E$2:$H$6, 3,FALSE)</f>
+        <v>300</v>
+      </c>
+      <c r="D12" s="22">
+        <f>SUMIF(Table4[Product], B12, Table4[Sales])</f>
+        <v>400</v>
+      </c>
+      <c r="E12" s="22">
+        <f>HLOOKUP(B12,$C$19:$G$21,3,FALSE)</f>
+        <v>300</v>
+      </c>
       <c r="J12" s="16">
         <v>5</v>
       </c>
@@ -6516,6 +8102,21 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="22">
+        <f>VLOOKUP(B13, $E$2:$H$6, 3, FALSE)</f>
+        <v>200</v>
+      </c>
+      <c r="D13" s="22">
+        <f>SUMIF(Table4[Product], B13, Table4[Sales])</f>
+        <v>200</v>
+      </c>
+      <c r="E13" s="22">
+        <f>HLOOKUP(B13,$C$19:$G$21,3,FALSE)</f>
+        <v>200</v>
+      </c>
       <c r="J13" s="16">
         <v>6</v>
       </c>
@@ -6528,7 +8129,7 @@
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="G14" s="21"/>
+      <c r="G14" s="20"/>
       <c r="J14" s="16">
         <v>7</v>
       </c>
@@ -6541,11 +8142,11 @@
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="G15" s="21"/>
+      <c r="G15" s="20"/>
       <c r="J15" s="16">
         <v>8</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" s="49" t="s">
         <v>25</v>
       </c>
       <c r="L15" s="3"/>
@@ -6557,7 +8158,7 @@
       <c r="J16" s="16">
         <v>9</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K16" s="48" t="s">
         <v>37</v>
       </c>
       <c r="L16" s="3"/>
@@ -6566,6 +8167,24 @@
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B17" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>48</v>
+      </c>
       <c r="J17" s="16">
         <v>10</v>
       </c>
@@ -6578,6 +8197,24 @@
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B18" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>9</v>
+      </c>
       <c r="J18" s="16">
         <v>11</v>
       </c>
@@ -6590,6 +8227,24 @@
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B19" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>13</v>
+      </c>
       <c r="J19" s="16">
         <v>12</v>
       </c>
@@ -6598,10 +8253,28 @@
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B20" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="41">
+        <v>30</v>
+      </c>
+      <c r="D20" s="41">
+        <v>25</v>
+      </c>
+      <c r="E20" s="41">
+        <v>20</v>
+      </c>
+      <c r="F20" s="41">
+        <v>15</v>
+      </c>
+      <c r="G20" s="41">
+        <v>10</v>
+      </c>
       <c r="J20" s="16">
         <v>13</v>
       </c>
@@ -6610,10 +8283,28 @@
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B21" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="41">
+        <v>300</v>
+      </c>
+      <c r="D21" s="41">
+        <v>250</v>
+      </c>
+      <c r="E21" s="41">
+        <v>200</v>
+      </c>
+      <c r="F21" s="41">
+        <v>150</v>
+      </c>
+      <c r="G21" s="41">
+        <v>100</v>
+      </c>
       <c r="J21" s="16">
         <v>14</v>
       </c>
@@ -6622,7 +8313,7 @@
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.35">
@@ -6634,7 +8325,7 @@
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.35">
@@ -6646,7 +8337,7 @@
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.35">
@@ -6658,7 +8349,7 @@
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.35">
@@ -6670,7 +8361,7 @@
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.35">
@@ -6686,7 +8377,7 @@
       </c>
     </row>
     <row r="27" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="30" t="s">
         <v>39</v>
       </c>
       <c r="C27" t="s">
@@ -6698,7 +8389,7 @@
       <c r="J27" s="17"/>
       <c r="K27" s="4"/>
       <c r="L27" s="5"/>
-      <c r="M27" s="13" t="b">
+      <c r="M27" s="47" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6706,38 +8397,32 @@
       <c r="B28" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28">
         <v>15</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28">
         <v>150</v>
-      </c>
-      <c r="M28" s="3" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B29" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="18">
+      <c r="C29">
         <v>15</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29">
         <v>150</v>
-      </c>
-      <c r="M29" s="3" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30">
         <v>40</v>
       </c>
-      <c r="D30" s="18">
+      <c r="D30">
         <v>400</v>
       </c>
       <c r="P30" s="5"/>
@@ -6746,10 +8431,10 @@
       <c r="B31" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31">
         <v>40</v>
       </c>
-      <c r="D31" s="18">
+      <c r="D31">
         <v>400</v>
       </c>
     </row>
@@ -6757,86 +8442,206 @@
       <c r="B32" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32">
         <v>20</v>
       </c>
-      <c r="D32" s="18">
+      <c r="D32">
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B33" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="18">
+      <c r="C33">
         <v>20</v>
       </c>
-      <c r="D33" s="18">
+      <c r="D33">
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="18">
+      <c r="C34">
         <v>25</v>
       </c>
-      <c r="D34" s="18">
+      <c r="D34">
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B35" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35">
         <v>25</v>
       </c>
-      <c r="D35" s="18">
+      <c r="D35">
         <v>250</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B36" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="18">
+      <c r="C36">
         <v>100</v>
       </c>
-      <c r="D36" s="18">
+      <c r="D36">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E42" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="45"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E44" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="F44" s="43">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E45" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="F45" s="43">
+        <v>35.355339059327378</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E46" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="F46" s="43">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E47" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="F47" s="43" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E48" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="F48" s="43">
+        <v>79.05694150420949</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E49" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="F49" s="43">
+        <v>6250</v>
+      </c>
+    </row>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E50" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="F50" s="43">
+        <v>-1.2000000000000046</v>
+      </c>
+    </row>
+    <row r="51" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E51" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F51" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E52" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" s="43">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E53" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="F53" s="43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E54" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="F54" s="43">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="55" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E55" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="F55" s="43">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="56" spans="5:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E56" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="F56" s="44">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:F6">
-    <sortCondition descending="1" ref="F2:F6"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:G6">
+    <sortCondition descending="1" ref="G2:G6"/>
   </sortState>
-  <conditionalFormatting sqref="K8:K26">
-    <cfRule type="expression" dxfId="20" priority="7">
-      <formula>M8=TRUE</formula>
+  <mergeCells count="2">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E42:F42"/>
+  </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="G2">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="greaterThan">
+      <formula>" £300.00 "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F6">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="G2:G6">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="greaterThan">
       <formula>200</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="greaterThan">
       <formula>" £200.00 "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="greaterThan">
       <formula>" £200.00"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThan">
       <formula>" £200.00 "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="greaterThan">
       <formula>" £200.00 "</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
-      <formula>" £300.00 "</formula>
+  <conditionalFormatting sqref="K8:K26">
+    <cfRule type="expression" dxfId="9" priority="14">
+      <formula>M8=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7270,4 +9075,71 @@
     <tablePart r:id="rId23"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0518F966-C039-4ADB-A21A-032884D46ABB}">
+  <dimension ref="A3:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="40">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="40">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="40">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="40">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="40">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>